<commit_message>
issue #494: add XLSX file reading
</commit_message>
<xml_diff>
--- a/core/src/test/resources/ti/excel/test.xlsx
+++ b/core/src/test/resources/ti/excel/test.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sole\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,24 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>test</t>
+    <t>titre1</t>
   </si>
   <si>
-    <t>jaune</t>
+    <t>titre2</t>
   </si>
   <si>
-    <t>bleu</t>
+    <t>titre 3</t>
   </si>
   <si>
-    <t>test2</t>
+    <t>2</t>
   </si>
   <si>
-    <t>vert</t>
-  </si>
-  <si>
-    <t>rouge</t>
+    <t>toto</t>
   </si>
 </sst>
 </file>
@@ -77,8 +70,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,7 +346,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -359,39 +354,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+      <c r="C3">
+        <f>3.7+B2</f>
+        <v>6.7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>